<commit_message>
Modificado el excel de ofertas asignaturas
Se ha añadido la columna mencion de la hoja optativas informatica
</commit_message>
<xml_diff>
--- a/Recursos/Oferta asignaturas.xlsx
+++ b/Recursos/Oferta asignaturas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Onieva\Google Drive\ABD\EnunciadosTrabajosGrupo\Secretaria2021\ParaAlumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\super\Documents\Universidad\Curso 20-21\Administracion Base de datos\Trabajo\Asignatura-305-Trabajo\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62C62B6-C8D7-42C2-9614-49393102D6FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10725" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Optativas_Informatica" sheetId="7" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="240">
   <si>
     <t>Ofertada</t>
   </si>
@@ -745,12 +746,15 @@
   </si>
   <si>
     <t>Matematicas</t>
+  </si>
+  <si>
+    <t>Informática</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -2315,118 +2319,118 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A1:L83" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:L83"/>
-  <sortState ref="A2:L83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla4" displayName="Tabla4" ref="A1:L83" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:L83" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L83">
     <sortCondition ref="D1:D83"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="Titulac." dataDxfId="52"/>
-    <tableColumn id="2" name="Ofertada" dataDxfId="51"/>
-    <tableColumn id="3" name="Cód." dataDxfId="50"/>
-    <tableColumn id="4" name="Referencia" dataDxfId="49"/>
-    <tableColumn id="5" name="Asignatura" dataDxfId="48"/>
-    <tableColumn id="6" name="Curso" dataDxfId="47"/>
-    <tableColumn id="7" name="Créd. teoría" dataDxfId="46"/>
-    <tableColumn id="8" name="Créd. práctica" dataDxfId="45"/>
-    <tableColumn id="9" name="Columna5" dataDxfId="44"/>
-    <tableColumn id="10" name="Duración" dataDxfId="43"/>
-    <tableColumn id="11" name="Plazas" dataDxfId="42"/>
-    <tableColumn id="12" name="Otro Idioma" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Titulac." dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ofertada" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cód." dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Referencia" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Asignatura" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Curso" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Créd. teoría" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Créd. práctica" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Columna5" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Duración" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Plazas" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Otro Idioma" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B1:L71" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="B1:L71"/>
-  <sortState ref="B2:L71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla3" displayName="Tabla3" ref="B1:L71" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="B1:L71" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L71">
     <sortCondition ref="D1:D71"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="Ofertada" dataDxfId="38"/>
-    <tableColumn id="2" name="Cód." dataDxfId="37"/>
-    <tableColumn id="3" name="Referencia" dataDxfId="36"/>
-    <tableColumn id="4" name="Asignatura" dataDxfId="35"/>
-    <tableColumn id="6" name="Curso" dataDxfId="34"/>
-    <tableColumn id="7" name="Créd. teoría" dataDxfId="33"/>
-    <tableColumn id="8" name="Créd. práctica" dataDxfId="32"/>
-    <tableColumn id="9" name="Columna5" dataDxfId="31"/>
-    <tableColumn id="10" name="Duración" dataDxfId="30"/>
-    <tableColumn id="11" name="Plazas" dataDxfId="29"/>
-    <tableColumn id="12" name="Otro Idioma" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Ofertada" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cód." dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Referencia" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Asignatura" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Curso" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Créd. teoría" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Créd. práctica" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Columna5" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Duración" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Plazas" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Otro Idioma" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:L71" totalsRowShown="0" headerRowDxfId="27">
-  <autoFilter ref="A1:L71"/>
-  <sortState ref="A2:L71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla2" displayName="Tabla2" ref="A1:L71" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="A1:L71" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L71">
     <sortCondition ref="D1:D71"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="Titulac."/>
-    <tableColumn id="2" name="Ofertada"/>
-    <tableColumn id="3" name="Cód."/>
-    <tableColumn id="4" name="Referencia"/>
-    <tableColumn id="5" name="Asignatura"/>
-    <tableColumn id="6" name="Curso"/>
-    <tableColumn id="7" name="Créd. teoría"/>
-    <tableColumn id="8" name="Créd. práctica"/>
-    <tableColumn id="9" name="Total créd."/>
-    <tableColumn id="10" name="Duración"/>
-    <tableColumn id="11" name="Plazas"/>
-    <tableColumn id="12" name="Otro Idioma"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Titulac."/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Ofertada"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cód."/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Referencia"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Asignatura"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Curso"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Créd. teoría"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Créd. práctica"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Total créd."/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Duración"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Plazas"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Otro Idioma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:K84" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:K84"/>
-  <sortState ref="A2:K84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabla1" displayName="Tabla1" ref="A1:K84" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:K84" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K84">
     <sortCondition ref="D1:D84"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="Titulac." dataDxfId="24"/>
-    <tableColumn id="2" name="Ofertada" dataDxfId="23"/>
-    <tableColumn id="3" name="Cód." dataDxfId="22"/>
-    <tableColumn id="5" name="Referencia" dataDxfId="21"/>
-    <tableColumn id="7" name="Asignatura" dataDxfId="20"/>
-    <tableColumn id="9" name="Curso" dataDxfId="19"/>
-    <tableColumn id="10" name="Créd. teoría" dataDxfId="18"/>
-    <tableColumn id="11" name="Créd. práctica" dataDxfId="17"/>
-    <tableColumn id="12" name="Total créditos" dataDxfId="16"/>
-    <tableColumn id="14" name="Duración" dataDxfId="15"/>
-    <tableColumn id="15" name="Plazas" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Titulac." dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Ofertada" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Cód." dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Referencia" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Asignatura" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Curso" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Créd. teoría" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Créd. práctica" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Total créditos" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="Duración" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="Plazas" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A1:L60" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L60"/>
-  <sortState ref="A2:L60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabla5" displayName="Tabla5" ref="A1:L60" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L60" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L60">
     <sortCondition ref="D1:D60"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="Titulac." dataDxfId="11"/>
-    <tableColumn id="2" name="Ofertada" dataDxfId="10"/>
-    <tableColumn id="3" name="Cód." dataDxfId="9"/>
-    <tableColumn id="4" name="Referencia" dataDxfId="8"/>
-    <tableColumn id="5" name="Asignatura" dataDxfId="7"/>
-    <tableColumn id="6" name="Curso" dataDxfId="6"/>
-    <tableColumn id="7" name="Créd. teoría" dataDxfId="5"/>
-    <tableColumn id="8" name="Créd. práctica" dataDxfId="4"/>
-    <tableColumn id="9" name="Columna5" dataDxfId="3"/>
-    <tableColumn id="10" name="Duración" dataDxfId="2"/>
-    <tableColumn id="11" name="Plazas" dataDxfId="1"/>
-    <tableColumn id="12" name="Otro Idioma" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Titulac." dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Ofertada" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Cód." dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Referencia" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Asignatura" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Curso" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Créd. teoría" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Créd. práctica" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Columna5" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Duración" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Plazas" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Otro Idioma" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2508,6 +2512,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2543,6 +2564,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2718,312 +2756,423 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="13"/>
+    <col min="2" max="2" width="11.44140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>235</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="10">
         <v>53158</v>
       </c>
       <c r="B2" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="10">
         <v>51047</v>
       </c>
       <c r="B3" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="10">
         <v>51031</v>
       </c>
       <c r="B4" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="10">
         <v>51006</v>
       </c>
       <c r="B5" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="10">
         <v>51035</v>
       </c>
       <c r="B6" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="10">
         <v>51051</v>
       </c>
       <c r="B7" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="10">
         <v>51018</v>
       </c>
       <c r="B8" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="10">
         <v>51019</v>
       </c>
       <c r="B9" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="10">
         <v>51010</v>
       </c>
       <c r="B10" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="10">
         <v>51057</v>
       </c>
       <c r="B11" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="10">
         <v>51012</v>
       </c>
       <c r="B12" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="10">
         <v>51042</v>
       </c>
       <c r="B13" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="10">
         <v>51014</v>
       </c>
       <c r="B14" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="10">
         <v>51044</v>
       </c>
       <c r="B15" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="10">
         <v>51026</v>
       </c>
       <c r="B16" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="10">
         <v>51030</v>
       </c>
       <c r="B17" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="10">
         <v>51730</v>
       </c>
       <c r="B18" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="10">
         <v>51190</v>
       </c>
       <c r="B19" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="10">
         <v>51191</v>
       </c>
       <c r="B20" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="10">
         <v>51192</v>
       </c>
       <c r="B21" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="10">
         <v>51048</v>
       </c>
       <c r="B22" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="10">
         <v>51049</v>
       </c>
       <c r="B23" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="10">
         <v>51050</v>
       </c>
       <c r="B24" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="10">
         <v>51734</v>
       </c>
       <c r="B25" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="10">
         <v>51052</v>
       </c>
       <c r="B26" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="10">
         <v>51020</v>
       </c>
       <c r="B27" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="10">
         <v>51053</v>
       </c>
       <c r="B28" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="10">
         <v>51021</v>
       </c>
       <c r="B29" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="10">
         <v>51056</v>
       </c>
       <c r="B30" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="10">
         <v>51039</v>
       </c>
       <c r="B31" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="10">
         <v>51040</v>
       </c>
       <c r="B32" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="10">
         <v>51023</v>
       </c>
       <c r="B33" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="10">
         <v>51054</v>
       </c>
       <c r="B34" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="10">
         <v>51738</v>
       </c>
       <c r="B35" s="12">
         <v>999</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="10">
         <v>51058</v>
       </c>
       <c r="B36" s="12">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="10">
         <v>51045</v>
       </c>
       <c r="B37" s="12">
         <v>999</v>
+      </c>
+      <c r="C37" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3032,14 +3181,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -3751,27 +3900,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7639,27 +7788,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10361,7 +10510,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A71"/>
+  <autoFilter ref="A1:A71" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -10371,26 +10520,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E36" sqref="E36:E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="4" width="6.88671875" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -13170,26 +13319,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -16143,27 +16292,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D31" sqref="D2:D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>